<commit_message>
added information in the docs folder
</commit_message>
<xml_diff>
--- a/docs/data_transformation_checks.xlsx
+++ b/docs/data_transformation_checks.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidsmith/Documents/Adobe/Deferred_Revenue_Forecast/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED912C01-B4A9-AB41-B2B9-657C1B7BC18C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EF3433A-4AEC-744F-AF8D-4244039F2D7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{2FC98428-676E-4246-9E45-E45D27046A0C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{2FC98428-676E-4246-9E45-E45D27046A0C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="USD_check" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +67,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">Total USD equivalent in the base booking file from this document currency (all periods)
 </t>
@@ -106,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{BECB7C77-1245-9B4A-8564-1DB33B890F0E}">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{BECB7C77-1245-9B4A-8564-1DB33B890F0E}">
       <text>
         <r>
           <rPr>
@@ -140,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB3" authorId="0" shapeId="0" xr:uid="{B8BD9EE4-3AD1-224B-B335-535F7D359F31}">
+    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{B8BD9EE4-3AD1-224B-B335-535F7D359F31}">
       <text>
         <r>
           <rPr>
@@ -173,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC3" authorId="0" shapeId="0" xr:uid="{F099AB22-9C20-B043-857A-1BDC87D7D4BD}">
+    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{F099AB22-9C20-B043-857A-1BDC87D7D4BD}">
       <text>
         <r>
           <rPr>
@@ -206,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD3" authorId="0" shapeId="0" xr:uid="{505625EB-6579-3D4A-8CC9-4B1E40243CEC}">
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{505625EB-6579-3D4A-8CC9-4B1E40243CEC}">
       <text>
         <r>
           <rPr>
@@ -239,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG3" authorId="0" shapeId="0" xr:uid="{A5A41EF0-1F67-A847-B549-5528BB37C01D}">
+    <comment ref="AD3" authorId="0" shapeId="0" xr:uid="{A5A41EF0-1F67-A847-B549-5528BB37C01D}">
       <text>
         <r>
           <rPr>
@@ -519,19 +519,18 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -676,9 +675,16 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -697,8 +703,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -708,20 +721,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,10 +736,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1040,55 +1035,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234F44FC-4D91-674B-825B-98D62928D6ED}">
-  <dimension ref="A2:AG42"/>
+  <dimension ref="A2:AD42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI37" sqref="AI37"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="D2" s="4" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="I2" s="7" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
-      <c r="O2" s="15" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="17"/>
-      <c r="W2" s="12" t="s">
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="14"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="22"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1110,134 +1105,134 @@
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="I3" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="J3" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="L3" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>62</v>
+      </c>
       <c r="O3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="S3" t="s">
-        <v>65</v>
-      </c>
-      <c r="T3" t="s">
-        <v>66</v>
-      </c>
-      <c r="U3" t="s">
         <v>40</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="T3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="X3" s="19" t="s">
+      <c r="U3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="Y3" s="19" t="s">
+      <c r="V3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="Z3" s="19" t="s">
+      <c r="W3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AA3" s="20" t="s">
+      <c r="X3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AB3" s="21" t="s">
+      <c r="Y3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AC3" s="22" t="s">
+      <c r="Z3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AD3" s="11" t="s">
+      <c r="AA3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AE3" s="11" t="s">
+      <c r="AB3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AD3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1379,9 +1374,9 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="O2:U2"/>
-    <mergeCell ref="W2:AE2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:S2"/>
+    <mergeCell ref="T2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>